<commit_message>
Add support for project dates
</commit_message>
<xml_diff>
--- a/worker/src/main/resources/by-developer.xlsx
+++ b/worker/src/main/resources/by-developer.xlsx
@@ -25,7 +25,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -39,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0">
+    <comment ref="A3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0">
+    <comment ref="A6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t xml:space="preserve">From (UTC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${report.start}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To (UTC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${report.end}</t>
+  </si>
   <si>
     <t xml:space="preserve">${developer.name}</t>
   </si>
@@ -103,32 +115,7 @@
     <t xml:space="preserve">${project.name} </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">${</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">project</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.duration}</t>
-    </r>
+    <t xml:space="preserve">${project.duration}</t>
   </si>
 </sst>
 </file>
@@ -165,20 +152,27 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF72BF44"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -227,7 +221,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,7 +230,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -244,11 +246,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -305,7 +307,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF72BF44"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -329,10 +331,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -349,53 +351,67 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="n">
-        <f aca="false">SUM(E2)</f>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <f aca="false">SUM(E3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>